<commit_message>
End of course back-up. PCA/UMAP
Much miscellany, but also Jonah Pearl's new unit on PCA and UMAP.
</commit_message>
<xml_diff>
--- a/Development/Effect of Height on Income/IncomeByHgtData.xlsx
+++ b/Development/Effect of Height on Income/IncomeByHgtData.xlsx
@@ -385,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C201"/>
+  <dimension ref="A1:D201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -396,7 +396,7 @@
     <col min="1" max="3" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -406,8 +406,9 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D1" s="2"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>67</v>
       </c>
@@ -418,7 +419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>69</v>
       </c>
@@ -429,7 +430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>68</v>
       </c>
@@ -440,7 +441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>63</v>
       </c>
@@ -451,7 +452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>70</v>
       </c>
@@ -462,7 +463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>66</v>
       </c>
@@ -473,7 +474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>67</v>
       </c>
@@ -484,7 +485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>68</v>
       </c>
@@ -495,7 +496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>64</v>
       </c>
@@ -506,7 +507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>68</v>
       </c>
@@ -517,7 +518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>62</v>
       </c>
@@ -528,7 +529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>65</v>
       </c>
@@ -539,7 +540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>70</v>
       </c>
@@ -550,7 +551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>69</v>
       </c>
@@ -561,7 +562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>67</v>
       </c>

</xml_diff>